<commit_message>
HDFCDEMO-9 #comment test #In_Progress
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Some Data here</t>
+    <t>Some more Data here</t>
   </si>
 </sst>
 </file>
@@ -360,10 +360,13 @@
   <dimension ref="A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>